<commit_message>
Update Readme.md and delete ipynb file
</commit_message>
<xml_diff>
--- a/save_accuracy.xlsx
+++ b/save_accuracy.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2178"/>
+  <dimension ref="A1:F2188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47823,7 +47823,7 @@
         <v>100</v>
       </c>
       <c r="F2154" t="n">
-        <v>75.81290435791016</v>
+        <v>79.06964874267578</v>
       </c>
     </row>
     <row r="2155">
@@ -47845,7 +47845,7 @@
         <v>200</v>
       </c>
       <c r="F2155" t="n">
-        <v>81.84429168701172</v>
+        <v>82.64950561523438</v>
       </c>
     </row>
     <row r="2156">
@@ -47867,7 +47867,7 @@
         <v>300</v>
       </c>
       <c r="F2156" t="n">
-        <v>83.66499328613281</v>
+        <v>83.35726928710938</v>
       </c>
     </row>
     <row r="2157">
@@ -47889,7 +47889,7 @@
         <v>400</v>
       </c>
       <c r="F2157" t="n">
-        <v>82.15201568603516</v>
+        <v>84.98307800292969</v>
       </c>
     </row>
     <row r="2158">
@@ -47911,7 +47911,7 @@
         <v>500</v>
       </c>
       <c r="F2158" t="n">
-        <v>84.47533416748047</v>
+        <v>84.98820495605469</v>
       </c>
     </row>
     <row r="2159">
@@ -47933,7 +47933,7 @@
         <v>600</v>
       </c>
       <c r="F2159" t="n">
-        <v>84.64457702636719</v>
+        <v>85.49081420898438</v>
       </c>
     </row>
     <row r="2160">
@@ -47955,7 +47955,7 @@
         <v>700</v>
       </c>
       <c r="F2160" t="n">
-        <v>85.86521911621094</v>
+        <v>86.11652374267578</v>
       </c>
     </row>
     <row r="2161">
@@ -47977,7 +47977,7 @@
         <v>800</v>
       </c>
       <c r="F2161" t="n">
-        <v>85.48568725585938</v>
+        <v>85.82418823242188</v>
       </c>
     </row>
     <row r="2162">
@@ -47999,7 +47999,7 @@
         <v>900</v>
       </c>
       <c r="F2162" t="n">
-        <v>86.62939453125</v>
+        <v>87.04482269287109</v>
       </c>
     </row>
     <row r="2163">
@@ -48021,7 +48021,7 @@
         <v>1000</v>
       </c>
       <c r="F2163" t="n">
-        <v>86.79351806640625</v>
+        <v>87.23971557617188</v>
       </c>
     </row>
     <row r="2164">
@@ -48043,7 +48043,7 @@
         <v>1100</v>
       </c>
       <c r="F2164" t="n">
-        <v>86.59862518310547</v>
+        <v>87.18330383300781</v>
       </c>
     </row>
     <row r="2165">
@@ -48065,7 +48065,7 @@
         <v>1200</v>
       </c>
       <c r="F2165" t="n">
-        <v>87.36793518066406</v>
+        <v>85.74725341796875</v>
       </c>
     </row>
     <row r="2166">
@@ -48087,7 +48087,7 @@
         <v>1300</v>
       </c>
       <c r="F2166" t="n">
-        <v>86.99353790283203</v>
+        <v>87.61411285400391</v>
       </c>
     </row>
     <row r="2167">
@@ -48109,7 +48109,7 @@
         <v>1400</v>
       </c>
       <c r="F2167" t="n">
-        <v>87.32177734375</v>
+        <v>87.37818908691406</v>
       </c>
     </row>
     <row r="2168">
@@ -48131,7 +48131,7 @@
         <v>1500</v>
       </c>
       <c r="F2168" t="n">
-        <v>87.57308959960938</v>
+        <v>87.76797485351562</v>
       </c>
     </row>
     <row r="2169">
@@ -48153,7 +48153,7 @@
         <v>1600</v>
       </c>
       <c r="F2169" t="n">
-        <v>87.73720550537109</v>
+        <v>87.88593292236328</v>
       </c>
     </row>
     <row r="2170">
@@ -48175,7 +48175,7 @@
         <v>1700</v>
       </c>
       <c r="F2170" t="n">
-        <v>88.11160278320312</v>
+        <v>88.17827606201172</v>
       </c>
     </row>
     <row r="2171">
@@ -48197,7 +48197,7 @@
         <v>1800</v>
       </c>
       <c r="F2171" t="n">
-        <v>88.03466796875</v>
+        <v>88.36290740966797</v>
       </c>
     </row>
     <row r="2172">
@@ -48219,7 +48219,7 @@
         <v>1900</v>
       </c>
       <c r="F2172" t="n">
-        <v>88.13724517822266</v>
+        <v>88.52189636230469</v>
       </c>
     </row>
     <row r="2173">
@@ -48241,7 +48241,7 @@
         <v>2000</v>
       </c>
       <c r="F2173" t="n">
-        <v>87.90132141113281</v>
+        <v>88.14237213134766</v>
       </c>
     </row>
     <row r="2174">
@@ -48263,7 +48263,7 @@
         <v>2100</v>
       </c>
       <c r="F2174" t="n">
-        <v>88.41932678222656</v>
+        <v>88.56292724609375</v>
       </c>
     </row>
     <row r="2175">
@@ -48285,7 +48285,7 @@
         <v>2200</v>
       </c>
       <c r="F2175" t="n">
-        <v>88.49112701416016</v>
+        <v>88.732177734375</v>
       </c>
     </row>
     <row r="2176">
@@ -48307,7 +48307,7 @@
         <v>2300</v>
       </c>
       <c r="F2176" t="n">
-        <v>88.20391845703125</v>
+        <v>88.732177734375</v>
       </c>
     </row>
     <row r="2177">
@@ -48329,7 +48329,7 @@
         <v>2400</v>
       </c>
       <c r="F2177" t="n">
-        <v>88.79885101318359</v>
+        <v>88.96297454833984</v>
       </c>
     </row>
     <row r="2178">
@@ -48351,7 +48351,227 @@
         <v>2500</v>
       </c>
       <c r="F2178" t="n">
-        <v>88.732177734375</v>
+        <v>88.95271301269531</v>
+      </c>
+    </row>
+    <row r="2179">
+      <c r="A2179" s="1" t="n">
+        <v>2177</v>
+      </c>
+      <c r="B2179" t="inlineStr">
+        <is>
+          <t>M-CLIP/M-BERT-Base-ViT-B</t>
+        </is>
+      </c>
+      <c r="C2179" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="D2179" t="n">
+        <v>64</v>
+      </c>
+      <c r="E2179" t="n">
+        <v>2600</v>
+      </c>
+      <c r="F2179" t="n">
+        <v>88.93732452392578</v>
+      </c>
+    </row>
+    <row r="2180">
+      <c r="A2180" s="1" t="n">
+        <v>2178</v>
+      </c>
+      <c r="B2180" t="inlineStr">
+        <is>
+          <t>M-CLIP/M-BERT-Base-ViT-B</t>
+        </is>
+      </c>
+      <c r="C2180" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="D2180" t="n">
+        <v>64</v>
+      </c>
+      <c r="E2180" t="n">
+        <v>2700</v>
+      </c>
+      <c r="F2180" t="n">
+        <v>88.90142822265625</v>
+      </c>
+    </row>
+    <row r="2181">
+      <c r="A2181" s="1" t="n">
+        <v>2179</v>
+      </c>
+      <c r="B2181" t="inlineStr">
+        <is>
+          <t>M-CLIP/M-BERT-Base-ViT-B</t>
+        </is>
+      </c>
+      <c r="C2181" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="D2181" t="n">
+        <v>64</v>
+      </c>
+      <c r="E2181" t="n">
+        <v>2800</v>
+      </c>
+      <c r="F2181" t="n">
+        <v>89.18350219726562</v>
+      </c>
+    </row>
+    <row r="2182">
+      <c r="A2182" s="1" t="n">
+        <v>2180</v>
+      </c>
+      <c r="B2182" t="inlineStr">
+        <is>
+          <t>M-CLIP/M-BERT-Base-ViT-B</t>
+        </is>
+      </c>
+      <c r="C2182" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="D2182" t="n">
+        <v>64</v>
+      </c>
+      <c r="E2182" t="n">
+        <v>2900</v>
+      </c>
+      <c r="F2182" t="n">
+        <v>89.16299438476562</v>
+      </c>
+    </row>
+    <row r="2183">
+      <c r="A2183" s="1" t="n">
+        <v>2181</v>
+      </c>
+      <c r="B2183" t="inlineStr">
+        <is>
+          <t>M-CLIP/M-BERT-Base-ViT-B</t>
+        </is>
+      </c>
+      <c r="C2183" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="D2183" t="n">
+        <v>64</v>
+      </c>
+      <c r="E2183" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F2183" t="n">
+        <v>89.19889068603516</v>
+      </c>
+    </row>
+    <row r="2184">
+      <c r="A2184" s="1" t="n">
+        <v>2182</v>
+      </c>
+      <c r="B2184" t="inlineStr">
+        <is>
+          <t>M-CLIP/M-BERT-Base-ViT-B</t>
+        </is>
+      </c>
+      <c r="C2184" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="D2184" t="n">
+        <v>64</v>
+      </c>
+      <c r="E2184" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2184" t="n">
+        <v>79.27992248535156</v>
+      </c>
+    </row>
+    <row r="2185">
+      <c r="A2185" s="1" t="n">
+        <v>2183</v>
+      </c>
+      <c r="B2185" t="inlineStr">
+        <is>
+          <t>M-CLIP/M-BERT-Base-ViT-B</t>
+        </is>
+      </c>
+      <c r="C2185" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="D2185" t="n">
+        <v>64</v>
+      </c>
+      <c r="E2185" t="n">
+        <v>200</v>
+      </c>
+      <c r="F2185" t="n">
+        <v>81.07498168945312</v>
+      </c>
+    </row>
+    <row r="2186">
+      <c r="A2186" s="1" t="n">
+        <v>2184</v>
+      </c>
+      <c r="B2186" t="inlineStr">
+        <is>
+          <t>M-CLIP/M-BERT-Base-ViT-B</t>
+        </is>
+      </c>
+      <c r="C2186" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="D2186" t="n">
+        <v>64</v>
+      </c>
+      <c r="E2186" t="n">
+        <v>300</v>
+      </c>
+      <c r="F2186" t="n">
+        <v>83.23930358886719</v>
+      </c>
+    </row>
+    <row r="2187">
+      <c r="A2187" s="1" t="n">
+        <v>2185</v>
+      </c>
+      <c r="B2187" t="inlineStr">
+        <is>
+          <t>M-CLIP/M-BERT-Base-ViT-B</t>
+        </is>
+      </c>
+      <c r="C2187" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="D2187" t="n">
+        <v>64</v>
+      </c>
+      <c r="E2187" t="n">
+        <v>400</v>
+      </c>
+      <c r="F2187" t="n">
+        <v>84.48046112060547</v>
+      </c>
+    </row>
+    <row r="2188">
+      <c r="A2188" s="1" t="n">
+        <v>2186</v>
+      </c>
+      <c r="B2188" t="inlineStr">
+        <is>
+          <t>M-CLIP/M-BERT-Base-ViT-B</t>
+        </is>
+      </c>
+      <c r="C2188" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="D2188" t="n">
+        <v>64</v>
+      </c>
+      <c r="E2188" t="n">
+        <v>500</v>
+      </c>
+      <c r="F2188" t="n">
+        <v>83.27520751953125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>